<commit_message>
updating dataframe to include income status
</commit_message>
<xml_diff>
--- a/data/NGSscoping_dbv5.xlsx
+++ b/data/NGSscoping_dbv5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/christina_faust_glasgow_ac_uk/Documents/Stefano_Christina_shared/NGS scoping review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B01AF4DF-969D-46D5-9147-046D8E39C864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D440DFD-EF48-4C26-919C-ECB2D0344381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="740" windowWidth="13940" windowHeight="18380" xr2:uid="{F7EEB8B0-62BD-D841-8F4A-7E45EE424C35}"/>
   </bookViews>
@@ -25,13 +25,13 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="10973" r:id="rId6"/>
-    <pivotCache cacheId="10974" r:id="rId7"/>
-    <pivotCache cacheId="10975" r:id="rId8"/>
-    <pivotCache cacheId="10976" r:id="rId9"/>
-    <pivotCache cacheId="10977" r:id="rId10"/>
-    <pivotCache cacheId="10978" r:id="rId11"/>
-    <pivotCache cacheId="10979" r:id="rId12"/>
+    <pivotCache cacheId="16272" r:id="rId6"/>
+    <pivotCache cacheId="16273" r:id="rId7"/>
+    <pivotCache cacheId="16274" r:id="rId8"/>
+    <pivotCache cacheId="16275" r:id="rId9"/>
+    <pivotCache cacheId="16276" r:id="rId10"/>
+    <pivotCache cacheId="16277" r:id="rId11"/>
+    <pivotCache cacheId="16278" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -7699,359 +7699,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B7F20B32-EB1A-3C48-AB80-7DB6686D718C}" name="PivotTable8" cacheId="10976" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A55:B58" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of NUCLEIC_ACID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{498A8F1C-EAB8-864C-81EE-A1EFC50CF4E7}" name="PivotTable10" cacheId="10979" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A61:B64" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of PUBLIC_CODE" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C80BB3FE-CC16-D049-B978-D03E4545BE48}" name="PivotTable6" cacheId="10975" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="D12:E21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="9">
-        <item x="7"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of AGENT_TYPE" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="0">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="1">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5D57A72-9517-7647-9F1C-E3000EC5426A}" name="PivotTable7" cacheId="10977" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A48:B52" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of PRE-NGS_CULTURE" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0510414E-E0AD-364E-BB85-1962DB4A8BE9}" name="PivotTable9" cacheId="10978" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="L52:S58" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="7">
-        <item x="4"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
-      <items count="5">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="7">
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of PUBLIC_DATA" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1CB4EDE-8701-174F-8F01-8B502925009C}" name="PivotTable2" cacheId="10974" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1CB4EDE-8701-174F-8F01-8B502925009C}" name="PivotTable2" cacheId="16273" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="D3:E9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField name="STUDY_AIMS" axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
@@ -8115,8 +7763,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E54339A-1E2C-3C44-92AF-DB09E752C581}" name="PivotTable1" cacheId="10973" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9E54339A-1E2C-3C44-92AF-DB09E752C581}" name="PivotTable1" cacheId="16272" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B45" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
@@ -8311,6 +7959,358 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Count of SAMPLING_GEO" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B7F20B32-EB1A-3C48-AB80-7DB6686D718C}" name="PivotTable8" cacheId="16275" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A55:B58" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of NUCLEIC_ACID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{498A8F1C-EAB8-864C-81EE-A1EFC50CF4E7}" name="PivotTable10" cacheId="16278" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A61:B64" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of PUBLIC_CODE" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C80BB3FE-CC16-D049-B978-D03E4545BE48}" name="PivotTable6" cacheId="16274" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="D12:E21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="9">
+        <item x="7"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of AGENT_TYPE" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="0">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5D57A72-9517-7647-9F1C-E3000EC5426A}" name="PivotTable7" cacheId="16276" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A48:B52" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of PRE-NGS_CULTURE" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0510414E-E0AD-364E-BB85-1962DB4A8BE9}" name="PivotTable9" cacheId="16277" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="L52:S58" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="7">
+        <item x="4"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="descending">
+      <items count="5">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="7">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of PUBLIC_DATA" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>

</xml_diff>